<commit_message>
đã sửa lại 1 chút ở 2 file quỷ kia
</commit_message>
<xml_diff>
--- a/chi_tiet_nganh_dtu_2025.xlsx
+++ b/chi_tiet_nganh_dtu_2025.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="354">
   <si>
     <t>TT</t>
   </si>
@@ -926,7 +926,7 @@
     <t>Hệ thống Thông tin quản lý chuẩn CMU (Đạt kiểm định ABET)</t>
   </si>
   <si>
-    <t>418(CMU)</t>
+    <t>410(CMU)</t>
   </si>
   <si>
     <t>Ngành Quản trị Kinh doanh (PSU)</t>
@@ -975,42 +975,6 @@
   </si>
   <si>
     <t>107(CSU)</t>
-  </si>
-  <si>
-    <t>7480101 (LK)</t>
-  </si>
-  <si>
-    <t>Ngành Khoa học Máy tính (TROY)</t>
-  </si>
-  <si>
-    <t>Công nghệ thông tin TROY</t>
-  </si>
-  <si>
-    <t>102(TROY)</t>
-  </si>
-  <si>
-    <t>7340101 (LK)</t>
-  </si>
-  <si>
-    <t>Ngành Quản trị Kinh doanh (TROY)</t>
-  </si>
-  <si>
-    <t>Quản trị Kinh doanh TROY</t>
-  </si>
-  <si>
-    <t>400(TROY)</t>
-  </si>
-  <si>
-    <t>7810201 (LK)</t>
-  </si>
-  <si>
-    <t>Ngành Quản trị Khách sạn (TROY)</t>
-  </si>
-  <si>
-    <t>Quản trị Du lịch &amp; Khách sạn TROY</t>
-  </si>
-  <si>
-    <t>407(TROY)</t>
   </si>
   <si>
     <t>7340101 (HP)</t>
@@ -1137,7 +1101,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1154,6 +1118,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -1636,16 +1606,13 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1654,124 +1621,129 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -2246,10 +2218,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1"/>
@@ -2296,7 +2268,7 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -2316,7 +2288,7 @@
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -2336,7 +2308,7 @@
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -2356,7 +2328,7 @@
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -2376,7 +2348,7 @@
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>128</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -2396,7 +2368,7 @@
       <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -2416,7 +2388,7 @@
       <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -2436,7 +2408,7 @@
       <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -2456,7 +2428,7 @@
       <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -2476,7 +2448,7 @@
       <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -2496,7 +2468,7 @@
       <c r="D12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -2516,7 +2488,7 @@
       <c r="D13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -2536,7 +2508,7 @@
       <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -2556,7 +2528,7 @@
       <c r="D15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -2576,7 +2548,7 @@
       <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -2596,7 +2568,7 @@
       <c r="D17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>53</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -2616,7 +2588,7 @@
       <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
         <v>57</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -2636,7 +2608,7 @@
       <c r="D19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -2656,7 +2628,7 @@
       <c r="D20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="3" t="s">
         <v>63</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -2676,7 +2648,7 @@
       <c r="D21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="3" t="s">
         <v>67</v>
       </c>
       <c r="F21" s="2" t="s">
@@ -2696,7 +2668,7 @@
       <c r="D22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F22" s="2" t="s">
@@ -2716,7 +2688,7 @@
       <c r="D23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F23" s="2" t="s">
@@ -2736,7 +2708,7 @@
       <c r="D24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="3" t="s">
         <v>78</v>
       </c>
       <c r="F24" s="2" t="s">
@@ -2756,7 +2728,7 @@
       <c r="D25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="3" t="s">
         <v>82</v>
       </c>
       <c r="F25" s="2" t="s">
@@ -2776,7 +2748,7 @@
       <c r="D26" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="3" t="s">
         <v>85</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -2796,7 +2768,7 @@
       <c r="D27" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="3" t="s">
         <v>89</v>
       </c>
       <c r="F27" s="2" t="s">
@@ -2816,7 +2788,7 @@
       <c r="D28" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="3" t="s">
         <v>92</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -2836,7 +2808,7 @@
       <c r="D29" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="3" t="s">
         <v>96</v>
       </c>
       <c r="F29" s="2" t="s">
@@ -2856,7 +2828,7 @@
       <c r="D30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="3" t="s">
         <v>100</v>
       </c>
       <c r="F30" s="2" t="s">
@@ -2876,7 +2848,7 @@
       <c r="D31" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="3" t="s">
         <v>105</v>
       </c>
       <c r="F31" s="2" t="s">
@@ -2896,7 +2868,7 @@
       <c r="D32" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="3" t="s">
         <v>109</v>
       </c>
       <c r="F32" s="2" t="s">
@@ -2916,7 +2888,7 @@
       <c r="D33" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="3" t="s">
         <v>113</v>
       </c>
       <c r="F33" s="2" t="s">
@@ -2936,7 +2908,7 @@
       <c r="D34" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="3" t="s">
         <v>116</v>
       </c>
       <c r="F34" s="2" t="s">
@@ -2956,7 +2928,7 @@
       <c r="D35" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="3" t="s">
         <v>118</v>
       </c>
       <c r="F35" s="2" t="s">
@@ -2976,7 +2948,7 @@
       <c r="D36" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="3" t="s">
         <v>120</v>
       </c>
       <c r="F36" s="2" t="s">
@@ -2996,7 +2968,7 @@
       <c r="D37" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="3" t="s">
         <v>124</v>
       </c>
       <c r="F37" s="2" t="s">
@@ -3016,7 +2988,7 @@
       <c r="D38" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="3" t="s">
         <v>128</v>
       </c>
       <c r="F38" s="2" t="s">
@@ -3036,7 +3008,7 @@
       <c r="D39" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="3" t="s">
         <v>132</v>
       </c>
       <c r="F39" s="2" t="s">
@@ -3056,7 +3028,7 @@
       <c r="D40" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="3" t="s">
         <v>136</v>
       </c>
       <c r="F40" s="2" t="s">
@@ -3076,7 +3048,7 @@
       <c r="D41" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="3" t="s">
         <v>138</v>
       </c>
       <c r="F41" s="2" t="s">
@@ -3096,7 +3068,7 @@
       <c r="D42" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="3" t="s">
         <v>142</v>
       </c>
       <c r="F42" s="2" t="s">
@@ -3116,7 +3088,7 @@
       <c r="D43" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="3" t="s">
         <v>146</v>
       </c>
       <c r="F43" s="2" t="s">
@@ -3136,7 +3108,7 @@
       <c r="D44" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="3" t="s">
         <v>148</v>
       </c>
       <c r="F44" s="2" t="s">
@@ -3156,7 +3128,7 @@
       <c r="D45" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="3" t="s">
         <v>152</v>
       </c>
       <c r="F45" s="2" t="s">
@@ -3176,7 +3148,7 @@
       <c r="D46" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="3" t="s">
         <v>154</v>
       </c>
       <c r="F46" s="2" t="s">
@@ -3196,7 +3168,7 @@
       <c r="D47" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="3" t="s">
         <v>158</v>
       </c>
       <c r="F47" s="2" t="s">
@@ -3216,7 +3188,7 @@
       <c r="D48" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="3" t="s">
         <v>160</v>
       </c>
       <c r="F48" s="2" t="s">
@@ -3236,7 +3208,7 @@
       <c r="D49" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="3" t="s">
         <v>164</v>
       </c>
       <c r="F49" s="2" t="s">
@@ -3256,7 +3228,7 @@
       <c r="D50" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E50" s="3" t="s">
         <v>168</v>
       </c>
       <c r="F50" s="2" t="s">
@@ -3276,7 +3248,7 @@
       <c r="D51" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E51" s="3" t="s">
         <v>172</v>
       </c>
       <c r="F51" s="2" t="s">
@@ -3296,7 +3268,7 @@
       <c r="D52" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E52" s="3" t="s">
         <v>175</v>
       </c>
       <c r="F52" s="2" t="s">
@@ -3316,7 +3288,7 @@
       <c r="D53" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E53" s="3" t="s">
         <v>177</v>
       </c>
       <c r="F53" s="2" t="s">
@@ -3336,7 +3308,7 @@
       <c r="D54" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="3" t="s">
         <v>181</v>
       </c>
       <c r="F54" s="2" t="s">
@@ -3356,7 +3328,7 @@
       <c r="D55" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E55" s="3" t="s">
         <v>183</v>
       </c>
       <c r="F55" s="2" t="s">
@@ -3376,7 +3348,7 @@
       <c r="D56" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="3" t="s">
         <v>185</v>
       </c>
       <c r="F56" s="2" t="s">
@@ -3396,7 +3368,7 @@
       <c r="D57" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E57" s="3" t="s">
         <v>189</v>
       </c>
       <c r="F57" s="2" t="s">
@@ -3416,7 +3388,7 @@
       <c r="D58" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E58" s="3" t="s">
         <v>191</v>
       </c>
       <c r="F58" s="2" t="s">
@@ -3436,7 +3408,7 @@
       <c r="D59" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E59" s="3" t="s">
         <v>193</v>
       </c>
       <c r="F59" s="2" t="s">
@@ -3456,7 +3428,7 @@
       <c r="D60" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E60" s="3" t="s">
         <v>197</v>
       </c>
       <c r="F60" s="2" t="s">
@@ -3476,7 +3448,7 @@
       <c r="D61" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="3" t="s">
         <v>199</v>
       </c>
       <c r="F61" s="2" t="s">
@@ -3496,7 +3468,7 @@
       <c r="D62" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="E62" s="3" t="s">
         <v>201</v>
       </c>
       <c r="F62" s="2" t="s">
@@ -3516,7 +3488,7 @@
       <c r="D63" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E63" s="3" t="s">
         <v>205</v>
       </c>
       <c r="F63" s="2" t="s">
@@ -3536,7 +3508,7 @@
       <c r="D64" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E64" s="3" t="s">
         <v>209</v>
       </c>
       <c r="F64" s="2" t="s">
@@ -3556,7 +3528,7 @@
       <c r="D65" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F65" s="2" t="s">
@@ -3576,7 +3548,7 @@
       <c r="D66" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E66" s="3" t="s">
         <v>217</v>
       </c>
       <c r="F66" s="2" t="s">
@@ -3596,7 +3568,7 @@
       <c r="D67" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E67" s="3" t="s">
         <v>219</v>
       </c>
       <c r="F67" s="2" t="s">
@@ -3616,7 +3588,7 @@
       <c r="D68" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="E68" s="3" t="s">
         <v>223</v>
       </c>
       <c r="F68" s="2" t="s">
@@ -3636,7 +3608,7 @@
       <c r="D69" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E69" s="3" t="s">
         <v>227</v>
       </c>
       <c r="F69" s="2" t="s">
@@ -3656,7 +3628,7 @@
       <c r="D70" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E70" s="3" t="s">
         <v>229</v>
       </c>
       <c r="F70" s="2" t="s">
@@ -3676,7 +3648,7 @@
       <c r="D71" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E71" s="3" t="s">
         <v>233</v>
       </c>
       <c r="F71" s="2" t="s">
@@ -3696,7 +3668,7 @@
       <c r="D72" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="3" t="s">
         <v>237</v>
       </c>
       <c r="F72" s="2" t="s">
@@ -3716,7 +3688,7 @@
       <c r="D73" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="3" t="s">
         <v>240</v>
       </c>
       <c r="F73" s="2" t="s">
@@ -3736,7 +3708,7 @@
       <c r="D74" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E74" s="3" t="s">
         <v>244</v>
       </c>
       <c r="F74" s="2" t="s">
@@ -3756,7 +3728,7 @@
       <c r="D75" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="3" t="s">
         <v>246</v>
       </c>
       <c r="F75" s="2" t="s">
@@ -3776,7 +3748,7 @@
       <c r="D76" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E76" s="3" t="s">
         <v>248</v>
       </c>
       <c r="F76" s="2" t="s">
@@ -3796,7 +3768,7 @@
       <c r="D77" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E77" s="3" t="s">
         <v>250</v>
       </c>
       <c r="F77" s="2" t="s">
@@ -3816,7 +3788,7 @@
       <c r="D78" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" s="3" t="s">
         <v>252</v>
       </c>
       <c r="F78" s="2" t="s">
@@ -3836,7 +3808,7 @@
       <c r="D79" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E79" s="3" t="s">
         <v>254</v>
       </c>
       <c r="F79" s="2" t="s">
@@ -3853,17 +3825,17 @@
       <c r="C80" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D80" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E80" s="3" t="s">
         <v>258</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="81" ht="14.25" customHeight="1" spans="1:6">
+    <row r="81" ht="14.25" customHeight="1" spans="1:26">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -3876,14 +3848,34 @@
       <c r="D81" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="3" t="s">
         <v>262</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="82" ht="14.25" customHeight="1" spans="1:6">
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="5"/>
+      <c r="O81" s="5"/>
+      <c r="P81" s="5"/>
+      <c r="Q81" s="5"/>
+      <c r="R81" s="5"/>
+      <c r="S81" s="5"/>
+      <c r="T81" s="5"/>
+      <c r="U81" s="5"/>
+      <c r="V81" s="5"/>
+      <c r="W81" s="5"/>
+      <c r="X81" s="5"/>
+      <c r="Y81" s="5"/>
+      <c r="Z81" s="5"/>
+    </row>
+    <row r="82" ht="14.25" customHeight="1" spans="1:26">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -3896,14 +3888,34 @@
       <c r="D82" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="E82" s="3" t="s">
         <v>266</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="83" ht="14.25" customHeight="1" spans="1:6">
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="5"/>
+      <c r="O82" s="5"/>
+      <c r="P82" s="5"/>
+      <c r="Q82" s="5"/>
+      <c r="R82" s="5"/>
+      <c r="S82" s="5"/>
+      <c r="T82" s="5"/>
+      <c r="U82" s="5"/>
+      <c r="V82" s="5"/>
+      <c r="W82" s="5"/>
+      <c r="X82" s="5"/>
+      <c r="Y82" s="5"/>
+      <c r="Z82" s="5"/>
+    </row>
+    <row r="83" ht="14.25" customHeight="1" spans="1:26">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -3916,12 +3928,32 @@
       <c r="D83" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="E83" s="3" t="s">
         <v>270</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>238</v>
       </c>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5"/>
+      <c r="O83" s="5"/>
+      <c r="P83" s="5"/>
+      <c r="Q83" s="5"/>
+      <c r="R83" s="5"/>
+      <c r="S83" s="5"/>
+      <c r="T83" s="5"/>
+      <c r="U83" s="5"/>
+      <c r="V83" s="5"/>
+      <c r="W83" s="5"/>
+      <c r="X83" s="5"/>
+      <c r="Y83" s="5"/>
+      <c r="Z83" s="5"/>
     </row>
     <row r="84" ht="14.25" customHeight="1" spans="1:26">
       <c r="A84" s="2">
@@ -3936,32 +3968,32 @@
       <c r="D84" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84" s="3">
         <v>305</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3"/>
-      <c r="L84" s="3"/>
-      <c r="M84" s="3"/>
-      <c r="N84" s="3"/>
-      <c r="O84" s="3"/>
-      <c r="P84" s="3"/>
-      <c r="Q84" s="3"/>
-      <c r="R84" s="3"/>
-      <c r="S84" s="3"/>
-      <c r="T84" s="3"/>
-      <c r="U84" s="3"/>
-      <c r="V84" s="3"/>
-      <c r="W84" s="3"/>
-      <c r="X84" s="3"/>
-      <c r="Y84" s="3"/>
-      <c r="Z84" s="3"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
+      <c r="N84" s="5"/>
+      <c r="O84" s="5"/>
+      <c r="P84" s="5"/>
+      <c r="Q84" s="5"/>
+      <c r="R84" s="5"/>
+      <c r="S84" s="5"/>
+      <c r="T84" s="5"/>
+      <c r="U84" s="5"/>
+      <c r="V84" s="5"/>
+      <c r="W84" s="5"/>
+      <c r="X84" s="5"/>
+      <c r="Y84" s="5"/>
+      <c r="Z84" s="5"/>
     </row>
     <row r="85" ht="14.25" customHeight="1" spans="1:26">
       <c r="A85" s="2">
@@ -3976,32 +4008,32 @@
       <c r="D85" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85" s="3">
         <v>304</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
-      <c r="K85" s="3"/>
-      <c r="L85" s="3"/>
-      <c r="M85" s="3"/>
-      <c r="N85" s="3"/>
-      <c r="O85" s="3"/>
-      <c r="P85" s="3"/>
-      <c r="Q85" s="3"/>
-      <c r="R85" s="3"/>
-      <c r="S85" s="3"/>
-      <c r="T85" s="3"/>
-      <c r="U85" s="3"/>
-      <c r="V85" s="3"/>
-      <c r="W85" s="3"/>
-      <c r="X85" s="3"/>
-      <c r="Y85" s="3"/>
-      <c r="Z85" s="3"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
+      <c r="N85" s="5"/>
+      <c r="O85" s="5"/>
+      <c r="P85" s="5"/>
+      <c r="Q85" s="5"/>
+      <c r="R85" s="5"/>
+      <c r="S85" s="5"/>
+      <c r="T85" s="5"/>
+      <c r="U85" s="5"/>
+      <c r="V85" s="5"/>
+      <c r="W85" s="5"/>
+      <c r="X85" s="5"/>
+      <c r="Y85" s="5"/>
+      <c r="Z85" s="5"/>
     </row>
     <row r="86" ht="14.25" customHeight="1" spans="1:26">
       <c r="A86" s="2">
@@ -4016,32 +4048,32 @@
       <c r="D86" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E86" s="2">
+      <c r="E86" s="3">
         <v>302</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
-      <c r="M86" s="3"/>
-      <c r="N86" s="3"/>
-      <c r="O86" s="3"/>
-      <c r="P86" s="3"/>
-      <c r="Q86" s="3"/>
-      <c r="R86" s="3"/>
-      <c r="S86" s="3"/>
-      <c r="T86" s="3"/>
-      <c r="U86" s="3"/>
-      <c r="V86" s="3"/>
-      <c r="W86" s="3"/>
-      <c r="X86" s="3"/>
-      <c r="Y86" s="3"/>
-      <c r="Z86" s="3"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+      <c r="M86" s="5"/>
+      <c r="N86" s="5"/>
+      <c r="O86" s="5"/>
+      <c r="P86" s="5"/>
+      <c r="Q86" s="5"/>
+      <c r="R86" s="5"/>
+      <c r="S86" s="5"/>
+      <c r="T86" s="5"/>
+      <c r="U86" s="5"/>
+      <c r="V86" s="5"/>
+      <c r="W86" s="5"/>
+      <c r="X86" s="5"/>
+      <c r="Y86" s="5"/>
+      <c r="Z86" s="5"/>
     </row>
     <row r="87" ht="14.25" customHeight="1" spans="1:26">
       <c r="A87" s="2">
@@ -4056,32 +4088,32 @@
       <c r="D87" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87" s="3">
         <v>303</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3"/>
-      <c r="K87" s="3"/>
-      <c r="L87" s="3"/>
-      <c r="M87" s="3"/>
-      <c r="N87" s="3"/>
-      <c r="O87" s="3"/>
-      <c r="P87" s="3"/>
-      <c r="Q87" s="3"/>
-      <c r="R87" s="3"/>
-      <c r="S87" s="3"/>
-      <c r="T87" s="3"/>
-      <c r="U87" s="3"/>
-      <c r="V87" s="3"/>
-      <c r="W87" s="3"/>
-      <c r="X87" s="3"/>
-      <c r="Y87" s="3"/>
-      <c r="Z87" s="3"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="5"/>
+      <c r="N87" s="5"/>
+      <c r="O87" s="5"/>
+      <c r="P87" s="5"/>
+      <c r="Q87" s="5"/>
+      <c r="R87" s="5"/>
+      <c r="S87" s="5"/>
+      <c r="T87" s="5"/>
+      <c r="U87" s="5"/>
+      <c r="V87" s="5"/>
+      <c r="W87" s="5"/>
+      <c r="X87" s="5"/>
+      <c r="Y87" s="5"/>
+      <c r="Z87" s="5"/>
     </row>
     <row r="88" ht="14.25" customHeight="1" spans="1:26">
       <c r="A88" s="2">
@@ -4096,32 +4128,32 @@
       <c r="D88" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88" s="3">
         <v>310</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
-      <c r="L88" s="3"/>
-      <c r="M88" s="3"/>
-      <c r="N88" s="3"/>
-      <c r="O88" s="3"/>
-      <c r="P88" s="3"/>
-      <c r="Q88" s="3"/>
-      <c r="R88" s="3"/>
-      <c r="S88" s="3"/>
-      <c r="T88" s="3"/>
-      <c r="U88" s="3"/>
-      <c r="V88" s="3"/>
-      <c r="W88" s="3"/>
-      <c r="X88" s="3"/>
-      <c r="Y88" s="3"/>
-      <c r="Z88" s="3"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="5"/>
+      <c r="N88" s="5"/>
+      <c r="O88" s="5"/>
+      <c r="P88" s="5"/>
+      <c r="Q88" s="5"/>
+      <c r="R88" s="5"/>
+      <c r="S88" s="5"/>
+      <c r="T88" s="5"/>
+      <c r="U88" s="5"/>
+      <c r="V88" s="5"/>
+      <c r="W88" s="5"/>
+      <c r="X88" s="5"/>
+      <c r="Y88" s="5"/>
+      <c r="Z88" s="5"/>
     </row>
     <row r="89" ht="14.25" customHeight="1" spans="1:26">
       <c r="A89" s="2">
@@ -4136,32 +4168,32 @@
       <c r="D89" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89" s="3">
         <v>320</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
-      <c r="I89" s="3"/>
-      <c r="J89" s="3"/>
-      <c r="K89" s="3"/>
-      <c r="L89" s="3"/>
-      <c r="M89" s="3"/>
-      <c r="N89" s="3"/>
-      <c r="O89" s="3"/>
-      <c r="P89" s="3"/>
-      <c r="Q89" s="3"/>
-      <c r="R89" s="3"/>
-      <c r="S89" s="3"/>
-      <c r="T89" s="3"/>
-      <c r="U89" s="3"/>
-      <c r="V89" s="3"/>
-      <c r="W89" s="3"/>
-      <c r="X89" s="3"/>
-      <c r="Y89" s="3"/>
-      <c r="Z89" s="3"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5"/>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+      <c r="L89" s="5"/>
+      <c r="M89" s="5"/>
+      <c r="N89" s="5"/>
+      <c r="O89" s="5"/>
+      <c r="P89" s="5"/>
+      <c r="Q89" s="5"/>
+      <c r="R89" s="5"/>
+      <c r="S89" s="5"/>
+      <c r="T89" s="5"/>
+      <c r="U89" s="5"/>
+      <c r="V89" s="5"/>
+      <c r="W89" s="5"/>
+      <c r="X89" s="5"/>
+      <c r="Y89" s="5"/>
+      <c r="Z89" s="5"/>
     </row>
     <row r="90" ht="14.25" customHeight="1" spans="1:26">
       <c r="A90" s="2">
@@ -4176,32 +4208,32 @@
       <c r="D90" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90" s="3">
         <v>330</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
-      <c r="L90" s="3"/>
-      <c r="M90" s="3"/>
-      <c r="N90" s="3"/>
-      <c r="O90" s="3"/>
-      <c r="P90" s="3"/>
-      <c r="Q90" s="3"/>
-      <c r="R90" s="3"/>
-      <c r="S90" s="3"/>
-      <c r="T90" s="3"/>
-      <c r="U90" s="3"/>
-      <c r="V90" s="3"/>
-      <c r="W90" s="3"/>
-      <c r="X90" s="3"/>
-      <c r="Y90" s="3"/>
-      <c r="Z90" s="3"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="5"/>
+      <c r="M90" s="5"/>
+      <c r="N90" s="5"/>
+      <c r="O90" s="5"/>
+      <c r="P90" s="5"/>
+      <c r="Q90" s="5"/>
+      <c r="R90" s="5"/>
+      <c r="S90" s="5"/>
+      <c r="T90" s="5"/>
+      <c r="U90" s="5"/>
+      <c r="V90" s="5"/>
+      <c r="W90" s="5"/>
+      <c r="X90" s="5"/>
+      <c r="Y90" s="5"/>
+      <c r="Z90" s="5"/>
     </row>
     <row r="91" ht="14.25" customHeight="1" spans="1:26">
       <c r="A91" s="2">
@@ -4216,32 +4248,32 @@
       <c r="D91" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="E91" s="3" t="s">
         <v>292</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G91" s="3"/>
-      <c r="H91" s="3"/>
-      <c r="I91" s="3"/>
-      <c r="J91" s="3"/>
-      <c r="K91" s="3"/>
-      <c r="L91" s="3"/>
-      <c r="M91" s="3"/>
-      <c r="N91" s="3"/>
-      <c r="O91" s="3"/>
-      <c r="P91" s="3"/>
-      <c r="Q91" s="3"/>
-      <c r="R91" s="3"/>
-      <c r="S91" s="3"/>
-      <c r="T91" s="3"/>
-      <c r="U91" s="3"/>
-      <c r="V91" s="3"/>
-      <c r="W91" s="3"/>
-      <c r="X91" s="3"/>
-      <c r="Y91" s="3"/>
-      <c r="Z91" s="3"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="5"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="L91" s="5"/>
+      <c r="M91" s="5"/>
+      <c r="N91" s="5"/>
+      <c r="O91" s="5"/>
+      <c r="P91" s="5"/>
+      <c r="Q91" s="5"/>
+      <c r="R91" s="5"/>
+      <c r="S91" s="5"/>
+      <c r="T91" s="5"/>
+      <c r="U91" s="5"/>
+      <c r="V91" s="5"/>
+      <c r="W91" s="5"/>
+      <c r="X91" s="5"/>
+      <c r="Y91" s="5"/>
+      <c r="Z91" s="5"/>
     </row>
     <row r="92" ht="14.25" customHeight="1" spans="1:26">
       <c r="A92" s="2">
@@ -4256,32 +4288,32 @@
       <c r="D92" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E92" s="2" t="s">
+      <c r="E92" s="3" t="s">
         <v>295</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G92" s="3"/>
-      <c r="H92" s="3"/>
-      <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
-      <c r="K92" s="3"/>
-      <c r="L92" s="3"/>
-      <c r="M92" s="3"/>
-      <c r="N92" s="3"/>
-      <c r="O92" s="3"/>
-      <c r="P92" s="3"/>
-      <c r="Q92" s="3"/>
-      <c r="R92" s="3"/>
-      <c r="S92" s="3"/>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-      <c r="W92" s="3"/>
-      <c r="X92" s="3"/>
-      <c r="Y92" s="3"/>
-      <c r="Z92" s="3"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5"/>
+      <c r="M92" s="5"/>
+      <c r="N92" s="5"/>
+      <c r="O92" s="5"/>
+      <c r="P92" s="5"/>
+      <c r="Q92" s="5"/>
+      <c r="R92" s="5"/>
+      <c r="S92" s="5"/>
+      <c r="T92" s="5"/>
+      <c r="U92" s="5"/>
+      <c r="V92" s="5"/>
+      <c r="W92" s="5"/>
+      <c r="X92" s="5"/>
+      <c r="Y92" s="5"/>
+      <c r="Z92" s="5"/>
     </row>
     <row r="93" ht="14.25" customHeight="1" spans="1:26">
       <c r="A93" s="2">
@@ -4296,32 +4328,32 @@
       <c r="D93" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="E93" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G93" s="3"/>
-      <c r="H93" s="3"/>
-      <c r="I93" s="3"/>
-      <c r="J93" s="3"/>
-      <c r="K93" s="3"/>
-      <c r="L93" s="3"/>
-      <c r="M93" s="3"/>
-      <c r="N93" s="3"/>
-      <c r="O93" s="3"/>
-      <c r="P93" s="3"/>
-      <c r="Q93" s="3"/>
-      <c r="R93" s="3"/>
-      <c r="S93" s="3"/>
-      <c r="T93" s="3"/>
-      <c r="U93" s="3"/>
-      <c r="V93" s="3"/>
-      <c r="W93" s="3"/>
-      <c r="X93" s="3"/>
-      <c r="Y93" s="3"/>
-      <c r="Z93" s="3"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5"/>
+      <c r="M93" s="5"/>
+      <c r="N93" s="5"/>
+      <c r="O93" s="5"/>
+      <c r="P93" s="5"/>
+      <c r="Q93" s="5"/>
+      <c r="R93" s="5"/>
+      <c r="S93" s="5"/>
+      <c r="T93" s="5"/>
+      <c r="U93" s="5"/>
+      <c r="V93" s="5"/>
+      <c r="W93" s="5"/>
+      <c r="X93" s="5"/>
+      <c r="Y93" s="5"/>
+      <c r="Z93" s="5"/>
     </row>
     <row r="94" ht="14.25" customHeight="1" spans="1:26">
       <c r="A94" s="2">
@@ -4336,32 +4368,32 @@
       <c r="D94" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E94" s="2" t="s">
+      <c r="E94" s="3" t="s">
         <v>302</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
-      <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
-      <c r="K94" s="3"/>
-      <c r="L94" s="3"/>
-      <c r="M94" s="3"/>
-      <c r="N94" s="3"/>
-      <c r="O94" s="3"/>
-      <c r="P94" s="3"/>
-      <c r="Q94" s="3"/>
-      <c r="R94" s="3"/>
-      <c r="S94" s="3"/>
-      <c r="T94" s="3"/>
-      <c r="U94" s="3"/>
-      <c r="V94" s="3"/>
-      <c r="W94" s="3"/>
-      <c r="X94" s="3"/>
-      <c r="Y94" s="3"/>
-      <c r="Z94" s="3"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
+      <c r="M94" s="5"/>
+      <c r="N94" s="5"/>
+      <c r="O94" s="5"/>
+      <c r="P94" s="5"/>
+      <c r="Q94" s="5"/>
+      <c r="R94" s="5"/>
+      <c r="S94" s="5"/>
+      <c r="T94" s="5"/>
+      <c r="U94" s="5"/>
+      <c r="V94" s="5"/>
+      <c r="W94" s="5"/>
+      <c r="X94" s="5"/>
+      <c r="Y94" s="5"/>
+      <c r="Z94" s="5"/>
     </row>
     <row r="95" ht="14.25" customHeight="1" spans="1:26">
       <c r="A95" s="2">
@@ -4376,32 +4408,32 @@
       <c r="D95" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="E95" s="3" t="s">
         <v>305</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
-      <c r="J95" s="3"/>
-      <c r="K95" s="3"/>
-      <c r="L95" s="3"/>
-      <c r="M95" s="3"/>
-      <c r="N95" s="3"/>
-      <c r="O95" s="3"/>
-      <c r="P95" s="3"/>
-      <c r="Q95" s="3"/>
-      <c r="R95" s="3"/>
-      <c r="S95" s="3"/>
-      <c r="T95" s="3"/>
-      <c r="U95" s="3"/>
-      <c r="V95" s="3"/>
-      <c r="W95" s="3"/>
-      <c r="X95" s="3"/>
-      <c r="Y95" s="3"/>
-      <c r="Z95" s="3"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
+      <c r="M95" s="5"/>
+      <c r="N95" s="5"/>
+      <c r="O95" s="5"/>
+      <c r="P95" s="5"/>
+      <c r="Q95" s="5"/>
+      <c r="R95" s="5"/>
+      <c r="S95" s="5"/>
+      <c r="T95" s="5"/>
+      <c r="U95" s="5"/>
+      <c r="V95" s="5"/>
+      <c r="W95" s="5"/>
+      <c r="X95" s="5"/>
+      <c r="Y95" s="5"/>
+      <c r="Z95" s="5"/>
     </row>
     <row r="96" ht="14.25" customHeight="1" spans="1:26">
       <c r="A96" s="2">
@@ -4416,32 +4448,32 @@
       <c r="D96" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="E96" s="3" t="s">
         <v>308</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G96" s="3"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="3"/>
-      <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
-      <c r="N96" s="3"/>
-      <c r="O96" s="3"/>
-      <c r="P96" s="3"/>
-      <c r="Q96" s="3"/>
-      <c r="R96" s="3"/>
-      <c r="S96" s="3"/>
-      <c r="T96" s="3"/>
-      <c r="U96" s="3"/>
-      <c r="V96" s="3"/>
-      <c r="W96" s="3"/>
-      <c r="X96" s="3"/>
-      <c r="Y96" s="3"/>
-      <c r="Z96" s="3"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="5"/>
+      <c r="J96" s="5"/>
+      <c r="K96" s="5"/>
+      <c r="L96" s="5"/>
+      <c r="M96" s="5"/>
+      <c r="N96" s="5"/>
+      <c r="O96" s="5"/>
+      <c r="P96" s="5"/>
+      <c r="Q96" s="5"/>
+      <c r="R96" s="5"/>
+      <c r="S96" s="5"/>
+      <c r="T96" s="5"/>
+      <c r="U96" s="5"/>
+      <c r="V96" s="5"/>
+      <c r="W96" s="5"/>
+      <c r="X96" s="5"/>
+      <c r="Y96" s="5"/>
+      <c r="Z96" s="5"/>
     </row>
     <row r="97" ht="14.25" customHeight="1" spans="1:26">
       <c r="A97" s="2">
@@ -4456,32 +4488,32 @@
       <c r="D97" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="E97" s="3" t="s">
         <v>311</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="G97" s="3"/>
-      <c r="H97" s="3"/>
-      <c r="I97" s="3"/>
-      <c r="J97" s="3"/>
-      <c r="K97" s="3"/>
-      <c r="L97" s="3"/>
-      <c r="M97" s="3"/>
-      <c r="N97" s="3"/>
-      <c r="O97" s="3"/>
-      <c r="P97" s="3"/>
-      <c r="Q97" s="3"/>
-      <c r="R97" s="3"/>
-      <c r="S97" s="3"/>
-      <c r="T97" s="3"/>
-      <c r="U97" s="3"/>
-      <c r="V97" s="3"/>
-      <c r="W97" s="3"/>
-      <c r="X97" s="3"/>
-      <c r="Y97" s="3"/>
-      <c r="Z97" s="3"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+      <c r="L97" s="5"/>
+      <c r="M97" s="5"/>
+      <c r="N97" s="5"/>
+      <c r="O97" s="5"/>
+      <c r="P97" s="5"/>
+      <c r="Q97" s="5"/>
+      <c r="R97" s="5"/>
+      <c r="S97" s="5"/>
+      <c r="T97" s="5"/>
+      <c r="U97" s="5"/>
+      <c r="V97" s="5"/>
+      <c r="W97" s="5"/>
+      <c r="X97" s="5"/>
+      <c r="Y97" s="5"/>
+      <c r="Z97" s="5"/>
     </row>
     <row r="98" ht="14.25" customHeight="1" spans="1:26">
       <c r="A98" s="2">
@@ -4496,32 +4528,32 @@
       <c r="D98" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E98" s="2" t="s">
+      <c r="E98" s="3" t="s">
         <v>315</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="G98" s="3"/>
-      <c r="H98" s="3"/>
-      <c r="I98" s="3"/>
-      <c r="J98" s="3"/>
-      <c r="K98" s="3"/>
-      <c r="L98" s="3"/>
-      <c r="M98" s="3"/>
-      <c r="N98" s="3"/>
-      <c r="O98" s="3"/>
-      <c r="P98" s="3"/>
-      <c r="Q98" s="3"/>
-      <c r="R98" s="3"/>
-      <c r="S98" s="3"/>
-      <c r="T98" s="3"/>
-      <c r="U98" s="3"/>
-      <c r="V98" s="3"/>
-      <c r="W98" s="3"/>
-      <c r="X98" s="3"/>
-      <c r="Y98" s="3"/>
-      <c r="Z98" s="3"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5"/>
+      <c r="J98" s="5"/>
+      <c r="K98" s="5"/>
+      <c r="L98" s="5"/>
+      <c r="M98" s="5"/>
+      <c r="N98" s="5"/>
+      <c r="O98" s="5"/>
+      <c r="P98" s="5"/>
+      <c r="Q98" s="5"/>
+      <c r="R98" s="5"/>
+      <c r="S98" s="5"/>
+      <c r="T98" s="5"/>
+      <c r="U98" s="5"/>
+      <c r="V98" s="5"/>
+      <c r="W98" s="5"/>
+      <c r="X98" s="5"/>
+      <c r="Y98" s="5"/>
+      <c r="Z98" s="5"/>
     </row>
     <row r="99" ht="14.25" customHeight="1" spans="1:26">
       <c r="A99" s="2">
@@ -4536,32 +4568,32 @@
       <c r="D99" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="E99" s="2" t="s">
+      <c r="E99" s="3" t="s">
         <v>319</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G99" s="3"/>
-      <c r="H99" s="3"/>
-      <c r="I99" s="3"/>
-      <c r="J99" s="3"/>
-      <c r="K99" s="3"/>
-      <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="3"/>
-      <c r="P99" s="3"/>
-      <c r="Q99" s="3"/>
-      <c r="R99" s="3"/>
-      <c r="S99" s="3"/>
-      <c r="T99" s="3"/>
-      <c r="U99" s="3"/>
-      <c r="V99" s="3"/>
-      <c r="W99" s="3"/>
-      <c r="X99" s="3"/>
-      <c r="Y99" s="3"/>
-      <c r="Z99" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5"/>
+      <c r="J99" s="5"/>
+      <c r="K99" s="5"/>
+      <c r="L99" s="5"/>
+      <c r="M99" s="5"/>
+      <c r="N99" s="5"/>
+      <c r="O99" s="5"/>
+      <c r="P99" s="5"/>
+      <c r="Q99" s="5"/>
+      <c r="R99" s="5"/>
+      <c r="S99" s="5"/>
+      <c r="T99" s="5"/>
+      <c r="U99" s="5"/>
+      <c r="V99" s="5"/>
+      <c r="W99" s="5"/>
+      <c r="X99" s="5"/>
+      <c r="Y99" s="5"/>
+      <c r="Z99" s="5"/>
     </row>
     <row r="100" ht="14.25" customHeight="1" spans="1:26">
       <c r="A100" s="2">
@@ -4576,32 +4608,32 @@
       <c r="D100" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="E100" s="3" t="s">
         <v>323</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G100" s="3"/>
-      <c r="H100" s="3"/>
-      <c r="I100" s="3"/>
-      <c r="J100" s="3"/>
-      <c r="K100" s="3"/>
-      <c r="L100" s="3"/>
-      <c r="M100" s="3"/>
-      <c r="N100" s="3"/>
-      <c r="O100" s="3"/>
-      <c r="P100" s="3"/>
-      <c r="Q100" s="3"/>
-      <c r="R100" s="3"/>
-      <c r="S100" s="3"/>
-      <c r="T100" s="3"/>
-      <c r="U100" s="3"/>
-      <c r="V100" s="3"/>
-      <c r="W100" s="3"/>
-      <c r="X100" s="3"/>
-      <c r="Y100" s="3"/>
-      <c r="Z100" s="3"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5"/>
+      <c r="L100" s="5"/>
+      <c r="M100" s="5"/>
+      <c r="N100" s="5"/>
+      <c r="O100" s="5"/>
+      <c r="P100" s="5"/>
+      <c r="Q100" s="5"/>
+      <c r="R100" s="5"/>
+      <c r="S100" s="5"/>
+      <c r="T100" s="5"/>
+      <c r="U100" s="5"/>
+      <c r="V100" s="5"/>
+      <c r="W100" s="5"/>
+      <c r="X100" s="5"/>
+      <c r="Y100" s="5"/>
+      <c r="Z100" s="5"/>
     </row>
     <row r="101" ht="14.25" customHeight="1" spans="1:26">
       <c r="A101" s="2">
@@ -4616,32 +4648,32 @@
       <c r="D101" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E101" s="3" t="s">
         <v>327</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-      <c r="J101" s="3"/>
-      <c r="K101" s="3"/>
-      <c r="L101" s="3"/>
-      <c r="M101" s="3"/>
-      <c r="N101" s="3"/>
-      <c r="O101" s="3"/>
-      <c r="P101" s="3"/>
-      <c r="Q101" s="3"/>
-      <c r="R101" s="3"/>
-      <c r="S101" s="3"/>
-      <c r="T101" s="3"/>
-      <c r="U101" s="3"/>
-      <c r="V101" s="3"/>
-      <c r="W101" s="3"/>
-      <c r="X101" s="3"/>
-      <c r="Y101" s="3"/>
-      <c r="Z101" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+      <c r="I101" s="5"/>
+      <c r="J101" s="5"/>
+      <c r="K101" s="5"/>
+      <c r="L101" s="5"/>
+      <c r="M101" s="5"/>
+      <c r="N101" s="5"/>
+      <c r="O101" s="5"/>
+      <c r="P101" s="5"/>
+      <c r="Q101" s="5"/>
+      <c r="R101" s="5"/>
+      <c r="S101" s="5"/>
+      <c r="T101" s="5"/>
+      <c r="U101" s="5"/>
+      <c r="V101" s="5"/>
+      <c r="W101" s="5"/>
+      <c r="X101" s="5"/>
+      <c r="Y101" s="5"/>
+      <c r="Z101" s="5"/>
     </row>
     <row r="102" ht="14.25" customHeight="1" spans="1:26">
       <c r="A102" s="2">
@@ -4656,513 +4688,396 @@
       <c r="D102" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="E102" s="2" t="s">
+      <c r="E102" s="3" t="s">
         <v>331</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="3"/>
-      <c r="J102" s="3"/>
-      <c r="K102" s="3"/>
-      <c r="L102" s="3"/>
-      <c r="M102" s="3"/>
-      <c r="N102" s="3"/>
-      <c r="O102" s="3"/>
-      <c r="P102" s="3"/>
-      <c r="Q102" s="3"/>
-      <c r="R102" s="3"/>
-      <c r="S102" s="3"/>
-      <c r="T102" s="3"/>
-      <c r="U102" s="3"/>
-      <c r="V102" s="3"/>
-      <c r="W102" s="3"/>
-      <c r="X102" s="3"/>
-      <c r="Y102" s="3"/>
-      <c r="Z102" s="3"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="5"/>
+      <c r="J102" s="5"/>
+      <c r="K102" s="5"/>
+      <c r="L102" s="5"/>
+      <c r="M102" s="5"/>
+      <c r="N102" s="5"/>
+      <c r="O102" s="5"/>
+      <c r="P102" s="5"/>
+      <c r="Q102" s="5"/>
+      <c r="R102" s="5"/>
+      <c r="S102" s="5"/>
+      <c r="T102" s="5"/>
+      <c r="U102" s="5"/>
+      <c r="V102" s="5"/>
+      <c r="W102" s="5"/>
+      <c r="X102" s="5"/>
+      <c r="Y102" s="5"/>
+      <c r="Z102" s="5"/>
     </row>
     <row r="103" ht="14.25" customHeight="1" spans="1:26">
       <c r="A103" s="2">
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="E103" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>335</v>
-      </c>
       <c r="F103" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G103" s="3"/>
-      <c r="H103" s="3"/>
-      <c r="I103" s="3"/>
-      <c r="J103" s="3"/>
-      <c r="K103" s="3"/>
-      <c r="L103" s="3"/>
-      <c r="M103" s="3"/>
-      <c r="N103" s="3"/>
-      <c r="O103" s="3"/>
-      <c r="P103" s="3"/>
-      <c r="Q103" s="3"/>
-      <c r="R103" s="3"/>
-      <c r="S103" s="3"/>
-      <c r="T103" s="3"/>
-      <c r="U103" s="3"/>
-      <c r="V103" s="3"/>
-      <c r="W103" s="3"/>
-      <c r="X103" s="3"/>
-      <c r="Y103" s="3"/>
-      <c r="Z103" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="5"/>
+      <c r="J103" s="5"/>
+      <c r="K103" s="5"/>
+      <c r="L103" s="5"/>
+      <c r="M103" s="5"/>
+      <c r="N103" s="5"/>
+      <c r="O103" s="5"/>
+      <c r="P103" s="5"/>
+      <c r="Q103" s="5"/>
+      <c r="R103" s="5"/>
+      <c r="S103" s="5"/>
+      <c r="T103" s="5"/>
+      <c r="U103" s="5"/>
+      <c r="V103" s="5"/>
+      <c r="W103" s="5"/>
+      <c r="X103" s="5"/>
+      <c r="Y103" s="5"/>
+      <c r="Z103" s="5"/>
     </row>
     <row r="104" ht="14.25" customHeight="1" spans="1:26">
       <c r="A104" s="2">
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="F104" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G104" s="3"/>
-      <c r="H104" s="3"/>
-      <c r="I104" s="3"/>
-      <c r="J104" s="3"/>
-      <c r="K104" s="3"/>
-      <c r="L104" s="3"/>
-      <c r="M104" s="3"/>
-      <c r="N104" s="3"/>
-      <c r="O104" s="3"/>
-      <c r="P104" s="3"/>
-      <c r="Q104" s="3"/>
-      <c r="R104" s="3"/>
-      <c r="S104" s="3"/>
-      <c r="T104" s="3"/>
-      <c r="U104" s="3"/>
-      <c r="V104" s="3"/>
-      <c r="W104" s="3"/>
-      <c r="X104" s="3"/>
-      <c r="Y104" s="3"/>
-      <c r="Z104" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+      <c r="I104" s="5"/>
+      <c r="J104" s="5"/>
+      <c r="K104" s="5"/>
+      <c r="L104" s="5"/>
+      <c r="M104" s="5"/>
+      <c r="N104" s="5"/>
+      <c r="O104" s="5"/>
+      <c r="P104" s="5"/>
+      <c r="Q104" s="5"/>
+      <c r="R104" s="5"/>
+      <c r="S104" s="5"/>
+      <c r="T104" s="5"/>
+      <c r="U104" s="5"/>
+      <c r="V104" s="5"/>
+      <c r="W104" s="5"/>
+      <c r="X104" s="5"/>
+      <c r="Y104" s="5"/>
+      <c r="Z104" s="5"/>
     </row>
     <row r="105" ht="14.25" customHeight="1" spans="1:26">
       <c r="A105" s="2">
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>340</v>
+        <v>54</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>343</v>
+        <v>56</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>338</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G105" s="3"/>
-      <c r="H105" s="3"/>
-      <c r="I105" s="3"/>
-      <c r="J105" s="3"/>
-      <c r="K105" s="3"/>
-      <c r="L105" s="3"/>
-      <c r="M105" s="3"/>
-      <c r="N105" s="3"/>
-      <c r="O105" s="3"/>
-      <c r="P105" s="3"/>
-      <c r="Q105" s="3"/>
-      <c r="R105" s="3"/>
-      <c r="S105" s="3"/>
-      <c r="T105" s="3"/>
-      <c r="U105" s="3"/>
-      <c r="V105" s="3"/>
-      <c r="W105" s="3"/>
-      <c r="X105" s="3"/>
-      <c r="Y105" s="3"/>
-      <c r="Z105" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+      <c r="I105" s="5"/>
+      <c r="J105" s="5"/>
+      <c r="K105" s="5"/>
+      <c r="L105" s="5"/>
+      <c r="M105" s="5"/>
+      <c r="N105" s="5"/>
+      <c r="O105" s="5"/>
+      <c r="P105" s="5"/>
+      <c r="Q105" s="5"/>
+      <c r="R105" s="5"/>
+      <c r="S105" s="5"/>
+      <c r="T105" s="5"/>
+      <c r="U105" s="5"/>
+      <c r="V105" s="5"/>
+      <c r="W105" s="5"/>
+      <c r="X105" s="5"/>
+      <c r="Y105" s="5"/>
+      <c r="Z105" s="5"/>
     </row>
     <row r="106" ht="14.25" customHeight="1" spans="1:26">
       <c r="A106" s="2">
         <v>105</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>6</v>
+      <c r="B106" s="2">
+        <v>7510205</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>346</v>
+        <v>50</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>340</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G106" s="3"/>
-      <c r="H106" s="3"/>
-      <c r="I106" s="3"/>
-      <c r="J106" s="3"/>
-      <c r="K106" s="3"/>
-      <c r="L106" s="3"/>
-      <c r="M106" s="3"/>
-      <c r="N106" s="3"/>
-      <c r="O106" s="3"/>
-      <c r="P106" s="3"/>
-      <c r="Q106" s="3"/>
-      <c r="R106" s="3"/>
-      <c r="S106" s="3"/>
-      <c r="T106" s="3"/>
-      <c r="U106" s="3"/>
-      <c r="V106" s="3"/>
-      <c r="W106" s="3"/>
-      <c r="X106" s="3"/>
-      <c r="Y106" s="3"/>
-      <c r="Z106" s="3"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
+      <c r="L106" s="5"/>
+      <c r="M106" s="5"/>
+      <c r="N106" s="5"/>
+      <c r="O106" s="5"/>
+      <c r="P106" s="5"/>
+      <c r="Q106" s="5"/>
+      <c r="R106" s="5"/>
+      <c r="S106" s="5"/>
+      <c r="T106" s="5"/>
+      <c r="U106" s="5"/>
+      <c r="V106" s="5"/>
+      <c r="W106" s="5"/>
+      <c r="X106" s="5"/>
+      <c r="Y106" s="5"/>
+      <c r="Z106" s="5"/>
     </row>
     <row r="107" ht="14.25" customHeight="1" spans="1:26">
       <c r="A107" s="2">
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>348</v>
+        <v>88</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>342</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G107" s="3"/>
-      <c r="H107" s="3"/>
-      <c r="I107" s="3"/>
-      <c r="J107" s="3"/>
-      <c r="K107" s="3"/>
-      <c r="L107" s="3"/>
-      <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
-      <c r="O107" s="3"/>
-      <c r="P107" s="3"/>
-      <c r="Q107" s="3"/>
-      <c r="R107" s="3"/>
-      <c r="S107" s="3"/>
-      <c r="T107" s="3"/>
-      <c r="U107" s="3"/>
-      <c r="V107" s="3"/>
-      <c r="W107" s="3"/>
-      <c r="X107" s="3"/>
-      <c r="Y107" s="3"/>
-      <c r="Z107" s="3"/>
+        <v>312</v>
+      </c>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+      <c r="I107" s="5"/>
+      <c r="J107" s="5"/>
+      <c r="K107" s="5"/>
+      <c r="L107" s="5"/>
+      <c r="M107" s="5"/>
+      <c r="N107" s="5"/>
+      <c r="O107" s="5"/>
+      <c r="P107" s="5"/>
+      <c r="Q107" s="5"/>
+      <c r="R107" s="5"/>
+      <c r="S107" s="5"/>
+      <c r="T107" s="5"/>
+      <c r="U107" s="5"/>
+      <c r="V107" s="5"/>
+      <c r="W107" s="5"/>
+      <c r="X107" s="5"/>
+      <c r="Y107" s="5"/>
+      <c r="Z107" s="5"/>
     </row>
     <row r="108" ht="14.25" customHeight="1" spans="1:26">
       <c r="A108" s="2">
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>350</v>
+        <v>81</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>344</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G108" s="3"/>
-      <c r="H108" s="3"/>
-      <c r="I108" s="3"/>
-      <c r="J108" s="3"/>
-      <c r="K108" s="3"/>
-      <c r="L108" s="3"/>
-      <c r="M108" s="3"/>
-      <c r="N108" s="3"/>
-      <c r="O108" s="3"/>
-      <c r="P108" s="3"/>
-      <c r="Q108" s="3"/>
-      <c r="R108" s="3"/>
-      <c r="S108" s="3"/>
-      <c r="T108" s="3"/>
-      <c r="U108" s="3"/>
-      <c r="V108" s="3"/>
-      <c r="W108" s="3"/>
-      <c r="X108" s="3"/>
-      <c r="Y108" s="3"/>
-      <c r="Z108" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+      <c r="I108" s="5"/>
+      <c r="J108" s="5"/>
+      <c r="K108" s="5"/>
+      <c r="L108" s="5"/>
+      <c r="M108" s="5"/>
+      <c r="N108" s="5"/>
+      <c r="O108" s="5"/>
+      <c r="P108" s="5"/>
+      <c r="Q108" s="5"/>
+      <c r="R108" s="5"/>
+      <c r="S108" s="5"/>
+      <c r="T108" s="5"/>
+      <c r="U108" s="5"/>
+      <c r="V108" s="5"/>
+      <c r="W108" s="5"/>
+      <c r="X108" s="5"/>
+      <c r="Y108" s="5"/>
+      <c r="Z108" s="5"/>
     </row>
     <row r="109" ht="14.25" customHeight="1" spans="1:26">
       <c r="A109" s="2">
         <v>108</v>
       </c>
       <c r="B109" s="2">
-        <v>7510205</v>
+        <v>7210403</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>352</v>
+        <v>70</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>346</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G109" s="3"/>
-      <c r="H109" s="3"/>
-      <c r="I109" s="3"/>
-      <c r="J109" s="3"/>
-      <c r="K109" s="3"/>
-      <c r="L109" s="3"/>
-      <c r="M109" s="3"/>
-      <c r="N109" s="3"/>
-      <c r="O109" s="3"/>
-      <c r="P109" s="3"/>
-      <c r="Q109" s="3"/>
-      <c r="R109" s="3"/>
-      <c r="S109" s="3"/>
-      <c r="T109" s="3"/>
-      <c r="U109" s="3"/>
-      <c r="V109" s="3"/>
-      <c r="W109" s="3"/>
-      <c r="X109" s="3"/>
-      <c r="Y109" s="3"/>
-      <c r="Z109" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
+      <c r="I109" s="5"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="5"/>
+      <c r="L109" s="5"/>
+      <c r="M109" s="5"/>
+      <c r="N109" s="5"/>
+      <c r="O109" s="5"/>
+      <c r="P109" s="5"/>
+      <c r="Q109" s="5"/>
+      <c r="R109" s="5"/>
+      <c r="S109" s="5"/>
+      <c r="T109" s="5"/>
+      <c r="U109" s="5"/>
+      <c r="V109" s="5"/>
+      <c r="W109" s="5"/>
+      <c r="X109" s="5"/>
+      <c r="Y109" s="5"/>
+      <c r="Z109" s="5"/>
     </row>
     <row r="110" ht="14.25" customHeight="1" spans="1:26">
       <c r="A110" s="2">
         <v>109</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>86</v>
+      <c r="B110" s="2">
+        <v>7540101</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>349</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="G110" s="3"/>
-      <c r="H110" s="3"/>
-      <c r="I110" s="3"/>
-      <c r="J110" s="3"/>
-      <c r="K110" s="3"/>
-      <c r="L110" s="3"/>
-      <c r="M110" s="3"/>
-      <c r="N110" s="3"/>
-      <c r="O110" s="3"/>
-      <c r="P110" s="3"/>
-      <c r="Q110" s="3"/>
-      <c r="R110" s="3"/>
-      <c r="S110" s="3"/>
-      <c r="T110" s="3"/>
-      <c r="U110" s="3"/>
-      <c r="V110" s="3"/>
-      <c r="W110" s="3"/>
-      <c r="X110" s="3"/>
-      <c r="Y110" s="3"/>
-      <c r="Z110" s="3"/>
-    </row>
-    <row r="111" ht="14.25" customHeight="1" spans="1:26">
+        <v>350</v>
+      </c>
+      <c r="G110" s="5"/>
+      <c r="H110" s="5"/>
+      <c r="I110" s="5"/>
+      <c r="J110" s="5"/>
+      <c r="K110" s="5"/>
+      <c r="L110" s="5"/>
+      <c r="M110" s="5"/>
+      <c r="N110" s="5"/>
+      <c r="O110" s="5"/>
+      <c r="P110" s="5"/>
+      <c r="Q110" s="5"/>
+      <c r="R110" s="5"/>
+      <c r="S110" s="5"/>
+      <c r="T110" s="5"/>
+      <c r="U110" s="5"/>
+      <c r="V110" s="5"/>
+      <c r="W110" s="5"/>
+      <c r="X110" s="5"/>
+      <c r="Y110" s="5"/>
+      <c r="Z110" s="5"/>
+    </row>
+    <row r="111" ht="13" customHeight="1" spans="1:26">
       <c r="A111" s="2">
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>79</v>
+        <v>271</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>356</v>
+        <v>279</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>352</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G111" s="3"/>
-      <c r="H111" s="3"/>
-      <c r="I111" s="3"/>
-      <c r="J111" s="3"/>
-      <c r="K111" s="3"/>
-      <c r="L111" s="3"/>
-      <c r="M111" s="3"/>
-      <c r="N111" s="3"/>
-      <c r="O111" s="3"/>
-      <c r="P111" s="3"/>
-      <c r="Q111" s="3"/>
-      <c r="R111" s="3"/>
-      <c r="S111" s="3"/>
-      <c r="T111" s="3"/>
-      <c r="U111" s="3"/>
-      <c r="V111" s="3"/>
-      <c r="W111" s="3"/>
-      <c r="X111" s="3"/>
-      <c r="Y111" s="3"/>
-      <c r="Z111" s="3"/>
-    </row>
-    <row r="112" ht="14.25" customHeight="1" spans="1:26">
-      <c r="A112" s="2">
-        <v>111</v>
-      </c>
-      <c r="B112" s="2">
-        <v>7210403</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G112" s="3"/>
-      <c r="H112" s="3"/>
-      <c r="I112" s="3"/>
-      <c r="J112" s="3"/>
-      <c r="K112" s="3"/>
-      <c r="L112" s="3"/>
-      <c r="M112" s="3"/>
-      <c r="N112" s="3"/>
-      <c r="O112" s="3"/>
-      <c r="P112" s="3"/>
-      <c r="Q112" s="3"/>
-      <c r="R112" s="3"/>
-      <c r="S112" s="3"/>
-      <c r="T112" s="3"/>
-      <c r="U112" s="3"/>
-      <c r="V112" s="3"/>
-      <c r="W112" s="3"/>
-      <c r="X112" s="3"/>
-      <c r="Y112" s="3"/>
-      <c r="Z112" s="3"/>
-    </row>
-    <row r="113" ht="14.25" customHeight="1" spans="1:26">
-      <c r="A113" s="2">
-        <v>112</v>
-      </c>
-      <c r="B113" s="2">
-        <v>7540101</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="G113" s="3"/>
-      <c r="H113" s="3"/>
-      <c r="I113" s="3"/>
-      <c r="J113" s="3"/>
-      <c r="K113" s="3"/>
-      <c r="L113" s="3"/>
-      <c r="M113" s="3"/>
-      <c r="N113" s="3"/>
-      <c r="O113" s="3"/>
-      <c r="P113" s="3"/>
-      <c r="Q113" s="3"/>
-      <c r="R113" s="3"/>
-      <c r="S113" s="3"/>
-      <c r="T113" s="3"/>
-      <c r="U113" s="3"/>
-      <c r="V113" s="3"/>
-      <c r="W113" s="3"/>
-      <c r="X113" s="3"/>
-      <c r="Y113" s="3"/>
-      <c r="Z113" s="3"/>
-    </row>
-    <row r="114" ht="14.25" customHeight="1" spans="1:26">
-      <c r="A114" s="2">
-        <v>113</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="G114" s="3"/>
-      <c r="H114" s="3"/>
-      <c r="I114" s="3"/>
-      <c r="J114" s="3"/>
-      <c r="K114" s="3"/>
-      <c r="L114" s="3"/>
-      <c r="M114" s="3"/>
-      <c r="N114" s="3"/>
-      <c r="O114" s="3"/>
-      <c r="P114" s="3"/>
-      <c r="Q114" s="3"/>
-      <c r="R114" s="3"/>
-      <c r="S114" s="3"/>
-      <c r="T114" s="3"/>
-      <c r="U114" s="3"/>
-      <c r="V114" s="3"/>
-      <c r="W114" s="3"/>
-      <c r="X114" s="3"/>
-      <c r="Y114" s="3"/>
-      <c r="Z114" s="3"/>
-    </row>
+        <v>353</v>
+      </c>
+      <c r="G111" s="5"/>
+      <c r="H111" s="5"/>
+      <c r="I111" s="5"/>
+      <c r="J111" s="5"/>
+      <c r="K111" s="5"/>
+      <c r="L111" s="5"/>
+      <c r="M111" s="5"/>
+      <c r="N111" s="5"/>
+      <c r="O111" s="5"/>
+      <c r="P111" s="5"/>
+      <c r="Q111" s="5"/>
+      <c r="R111" s="5"/>
+      <c r="S111" s="5"/>
+      <c r="T111" s="5"/>
+      <c r="U111" s="5"/>
+      <c r="V111" s="5"/>
+      <c r="W111" s="5"/>
+      <c r="X111" s="5"/>
+      <c r="Y111" s="5"/>
+      <c r="Z111" s="5"/>
+    </row>
+    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="113" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1"/>
     <row r="115" ht="14.25" customHeight="1"/>
     <row r="116" ht="14.25" customHeight="1"/>
     <row r="117" ht="14.25" customHeight="1"/>
@@ -6046,10 +5961,10 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
+  <sortState ref="A2:F111">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="1" orientation="landscape"/>
   <headerFooter/>

</xml_diff>